<commit_message>
run readme python terminal
</commit_message>
<xml_diff>
--- a/cleaned_dataset.xlsx
+++ b/cleaned_dataset.xlsx
@@ -665,7 +665,7 @@
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>'new car'</t>
+          <t>new car</t>
         </is>
       </c>
       <c r="D6" t="n">
@@ -794,7 +794,7 @@
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>'used car'</t>
+          <t>used car</t>
         </is>
       </c>
       <c r="D9" t="n">
@@ -880,7 +880,7 @@
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>'new car'</t>
+          <t>new car</t>
         </is>
       </c>
       <c r="D11" t="n">
@@ -923,7 +923,7 @@
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>'new car'</t>
+          <t>new car</t>
         </is>
       </c>
       <c r="D12" t="n">
@@ -1052,7 +1052,7 @@
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>'new car'</t>
+          <t>new car</t>
         </is>
       </c>
       <c r="D15" t="n">
@@ -1095,7 +1095,7 @@
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>'new car'</t>
+          <t>new car</t>
         </is>
       </c>
       <c r="D16" t="n">
@@ -1267,7 +1267,7 @@
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>'used car'</t>
+          <t>used car</t>
         </is>
       </c>
       <c r="D20" t="n">
@@ -1353,7 +1353,7 @@
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>'new car'</t>
+          <t>new car</t>
         </is>
       </c>
       <c r="D22" t="n">
@@ -1439,7 +1439,7 @@
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>'new car'</t>
+          <t>new car</t>
         </is>
       </c>
       <c r="D24" t="n">
@@ -1482,7 +1482,7 @@
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>'used car'</t>
+          <t>used car</t>
         </is>
       </c>
       <c r="D25" t="n">
@@ -1869,7 +1869,7 @@
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>'new car'</t>
+          <t>new car</t>
         </is>
       </c>
       <c r="D34" t="n">
@@ -2127,7 +2127,7 @@
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>'domestic appliance'</t>
+          <t>domestic appliance</t>
         </is>
       </c>
       <c r="D40" t="n">
@@ -2342,7 +2342,7 @@
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>'used car'</t>
+          <t>used car</t>
         </is>
       </c>
       <c r="D45" t="n">
@@ -2385,7 +2385,7 @@
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>'used car'</t>
+          <t>used car</t>
         </is>
       </c>
       <c r="D46" t="n">
@@ -2428,7 +2428,7 @@
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>'new car'</t>
+          <t>new car</t>
         </is>
       </c>
       <c r="D47" t="n">
@@ -2514,7 +2514,7 @@
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>'used car'</t>
+          <t>used car</t>
         </is>
       </c>
       <c r="D49" t="n">
@@ -2557,7 +2557,7 @@
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>new car'</t>
+          <t>new car</t>
         </is>
       </c>
       <c r="D50" t="n">
@@ -2686,7 +2686,7 @@
       </c>
       <c r="C53" t="inlineStr">
         <is>
-          <t>use car'</t>
+          <t>used car</t>
         </is>
       </c>
       <c r="D53" t="n">
@@ -2772,7 +2772,7 @@
       </c>
       <c r="C55" t="inlineStr">
         <is>
-          <t>'used car'</t>
+          <t>used car</t>
         </is>
       </c>
       <c r="D55" t="n">
@@ -2815,7 +2815,7 @@
       </c>
       <c r="C56" t="inlineStr">
         <is>
-          <t>'new car'</t>
+          <t>new car</t>
         </is>
       </c>
       <c r="D56" t="n">
@@ -2858,7 +2858,7 @@
       </c>
       <c r="C57" t="inlineStr">
         <is>
-          <t>new car'</t>
+          <t>new car</t>
         </is>
       </c>
       <c r="D57" t="n">
@@ -2987,7 +2987,7 @@
       </c>
       <c r="C60" t="inlineStr">
         <is>
-          <t>'new car'</t>
+          <t>new car</t>
         </is>
       </c>
       <c r="D60" t="n">
@@ -3374,7 +3374,7 @@
       </c>
       <c r="C69" t="inlineStr">
         <is>
-          <t>'new car'</t>
+          <t>new car</t>
         </is>
       </c>
       <c r="D69" t="n">
@@ -3503,7 +3503,7 @@
       </c>
       <c r="C72" t="inlineStr">
         <is>
-          <t>'used car'</t>
+          <t>used car</t>
         </is>
       </c>
       <c r="D72" t="n">
@@ -3718,7 +3718,7 @@
       </c>
       <c r="C77" t="inlineStr">
         <is>
-          <t>'used car'</t>
+          <t>used car</t>
         </is>
       </c>
       <c r="D77" t="n">
@@ -3847,7 +3847,7 @@
       </c>
       <c r="C80" t="inlineStr">
         <is>
-          <t>'used car'</t>
+          <t>used car</t>
         </is>
       </c>
       <c r="D80" t="n">
@@ -4062,7 +4062,7 @@
       </c>
       <c r="C85" t="inlineStr">
         <is>
-          <t>the</t>
+          <t>other</t>
         </is>
       </c>
       <c r="D85" t="n">
@@ -4277,7 +4277,7 @@
       </c>
       <c r="C90" t="inlineStr">
         <is>
-          <t>'new car'</t>
+          <t>new car</t>
         </is>
       </c>
       <c r="D90" t="n">
@@ -4406,7 +4406,7 @@
       </c>
       <c r="C93" t="inlineStr">
         <is>
-          <t>'used car'</t>
+          <t>used car</t>
         </is>
       </c>
       <c r="D93" t="n">
@@ -4535,7 +4535,7 @@
       </c>
       <c r="C96" t="inlineStr">
         <is>
-          <t>'new car'</t>
+          <t>new car</t>
         </is>
       </c>
       <c r="D96" t="n">
@@ -4750,7 +4750,7 @@
       </c>
       <c r="C101" t="inlineStr">
         <is>
-          <t>'used car'</t>
+          <t>used car</t>
         </is>
       </c>
       <c r="D101" t="n">
@@ -4793,7 +4793,7 @@
       </c>
       <c r="C102" t="inlineStr">
         <is>
-          <t>'new car'</t>
+          <t>new car</t>
         </is>
       </c>
       <c r="D102" t="n">
@@ -4965,7 +4965,7 @@
       </c>
       <c r="C106" t="inlineStr">
         <is>
-          <t>'used car'</t>
+          <t>used car</t>
         </is>
       </c>
       <c r="D106" t="n">
@@ -5051,7 +5051,7 @@
       </c>
       <c r="C108" t="inlineStr">
         <is>
-          <t>'new car'</t>
+          <t>new car</t>
         </is>
       </c>
       <c r="D108" t="n">
@@ -5094,7 +5094,7 @@
       </c>
       <c r="C109" t="inlineStr">
         <is>
-          <t>'new car'</t>
+          <t>new car</t>
         </is>
       </c>
       <c r="D109" t="n">
@@ -5309,7 +5309,7 @@
       </c>
       <c r="C114" t="inlineStr">
         <is>
-          <t>'new car'</t>
+          <t>new car</t>
         </is>
       </c>
       <c r="D114" t="n">
@@ -5352,7 +5352,7 @@
       </c>
       <c r="C115" t="inlineStr">
         <is>
-          <t>'new car'</t>
+          <t>new car</t>
         </is>
       </c>
       <c r="D115" t="n">
@@ -5610,7 +5610,7 @@
       </c>
       <c r="C121" t="inlineStr">
         <is>
-          <t>'new car'</t>
+          <t>new car</t>
         </is>
       </c>
       <c r="D121" t="n">
@@ -5696,7 +5696,7 @@
       </c>
       <c r="C123" t="inlineStr">
         <is>
-          <t>'used car'</t>
+          <t>used car</t>
         </is>
       </c>
       <c r="D123" t="n">
@@ -5782,7 +5782,7 @@
       </c>
       <c r="C125" t="inlineStr">
         <is>
-          <t>'new car'</t>
+          <t>new car</t>
         </is>
       </c>
       <c r="D125" t="n">
@@ -5868,7 +5868,7 @@
       </c>
       <c r="C127" t="inlineStr">
         <is>
-          <t>'new car'</t>
+          <t>new car</t>
         </is>
       </c>
       <c r="D127" t="n">
@@ -5997,7 +5997,7 @@
       </c>
       <c r="C130" t="inlineStr">
         <is>
-          <t>'used car'</t>
+          <t>used car</t>
         </is>
       </c>
       <c r="D130" t="n">
@@ -6040,7 +6040,7 @@
       </c>
       <c r="C131" t="inlineStr">
         <is>
-          <t>'new car'</t>
+          <t>new car</t>
         </is>
       </c>
       <c r="D131" t="n">
@@ -6083,7 +6083,7 @@
       </c>
       <c r="C132" t="inlineStr">
         <is>
-          <t>'new car'</t>
+          <t>new car</t>
         </is>
       </c>
       <c r="D132" t="n">
@@ -6341,7 +6341,7 @@
       </c>
       <c r="C138" t="inlineStr">
         <is>
-          <t>'used car'</t>
+          <t>used car</t>
         </is>
       </c>
       <c r="D138" t="n">
@@ -6513,7 +6513,7 @@
       </c>
       <c r="C142" t="inlineStr">
         <is>
-          <t>'new car'</t>
+          <t>new car</t>
         </is>
       </c>
       <c r="D142" t="n">
@@ -6771,7 +6771,7 @@
       </c>
       <c r="C148" t="inlineStr">
         <is>
-          <t>'new car'</t>
+          <t>new car</t>
         </is>
       </c>
       <c r="D148" t="n">
@@ -6814,7 +6814,7 @@
       </c>
       <c r="C149" t="inlineStr">
         <is>
-          <t>'new car'</t>
+          <t>new car</t>
         </is>
       </c>
       <c r="D149" t="n">
@@ -7072,7 +7072,7 @@
       </c>
       <c r="C155" t="inlineStr">
         <is>
-          <t>'used car'</t>
+          <t>used car</t>
         </is>
       </c>
       <c r="D155" t="n">
@@ -7287,7 +7287,7 @@
       </c>
       <c r="C160" t="inlineStr">
         <is>
-          <t>'new car'</t>
+          <t>new car</t>
         </is>
       </c>
       <c r="D160" t="n">
@@ -7416,7 +7416,7 @@
       </c>
       <c r="C163" t="inlineStr">
         <is>
-          <t>'new car'</t>
+          <t>new car</t>
         </is>
       </c>
       <c r="D163" t="n">
@@ -7459,7 +7459,7 @@
       </c>
       <c r="C164" t="inlineStr">
         <is>
-          <t>'domestic appliance'</t>
+          <t>domestic appliance</t>
         </is>
       </c>
       <c r="D164" t="n">
@@ -7502,7 +7502,7 @@
       </c>
       <c r="C165" t="inlineStr">
         <is>
-          <t>'new car'</t>
+          <t>new car</t>
         </is>
       </c>
       <c r="D165" t="n">
@@ -7545,7 +7545,7 @@
       </c>
       <c r="C166" t="inlineStr">
         <is>
-          <t>'new car'</t>
+          <t>new car</t>
         </is>
       </c>
       <c r="D166" t="n">
@@ -7803,7 +7803,7 @@
       </c>
       <c r="C172" t="inlineStr">
         <is>
-          <t>'new car'</t>
+          <t>new car</t>
         </is>
       </c>
       <c r="D172" t="n">
@@ -8018,7 +8018,7 @@
       </c>
       <c r="C177" t="inlineStr">
         <is>
-          <t>'used car'</t>
+          <t>used car</t>
         </is>
       </c>
       <c r="D177" t="n">
@@ -8190,7 +8190,7 @@
       </c>
       <c r="C181" t="inlineStr">
         <is>
-          <t>'new car'</t>
+          <t>new car</t>
         </is>
       </c>
       <c r="D181" t="n">
@@ -8319,7 +8319,7 @@
       </c>
       <c r="C184" t="inlineStr">
         <is>
-          <t>'new car'</t>
+          <t>new car</t>
         </is>
       </c>
       <c r="D184" t="n">
@@ -8405,7 +8405,7 @@
       </c>
       <c r="C186" t="inlineStr">
         <is>
-          <t>'new car'</t>
+          <t>new car</t>
         </is>
       </c>
       <c r="D186" t="n">
@@ -8491,7 +8491,7 @@
       </c>
       <c r="C188" t="inlineStr">
         <is>
-          <t>use car'</t>
+          <t>used car</t>
         </is>
       </c>
       <c r="D188" t="n">
@@ -8534,7 +8534,7 @@
       </c>
       <c r="C189" t="inlineStr">
         <is>
-          <t>'new car'</t>
+          <t>new car</t>
         </is>
       </c>
       <c r="D189" t="n">
@@ -9007,7 +9007,7 @@
       </c>
       <c r="C200" t="inlineStr">
         <is>
-          <t>'used car'</t>
+          <t>used car</t>
         </is>
       </c>
       <c r="D200" t="n">
@@ -9136,7 +9136,7 @@
       </c>
       <c r="C203" t="inlineStr">
         <is>
-          <t>'new car'</t>
+          <t>new car</t>
         </is>
       </c>
       <c r="D203" t="n">
@@ -9265,7 +9265,7 @@
       </c>
       <c r="C206" t="inlineStr">
         <is>
-          <t>'new car'</t>
+          <t>new car</t>
         </is>
       </c>
       <c r="D206" t="n">
@@ -9308,7 +9308,7 @@
       </c>
       <c r="C207" t="inlineStr">
         <is>
-          <t>'used car'</t>
+          <t>used car</t>
         </is>
       </c>
       <c r="D207" t="n">
@@ -9394,7 +9394,7 @@
       </c>
       <c r="C209" t="inlineStr">
         <is>
-          <t>'domestic appliance'</t>
+          <t>domestic appliance</t>
         </is>
       </c>
       <c r="D209" t="n">
@@ -9480,7 +9480,7 @@
       </c>
       <c r="C211" t="inlineStr">
         <is>
-          <t>'used car'</t>
+          <t>used car</t>
         </is>
       </c>
       <c r="D211" t="n">
@@ -9910,7 +9910,7 @@
       </c>
       <c r="C221" t="inlineStr">
         <is>
-          <t>'new car'</t>
+          <t>new car</t>
         </is>
       </c>
       <c r="D221" t="n">
@@ -10125,7 +10125,7 @@
       </c>
       <c r="C226" t="inlineStr">
         <is>
-          <t>'used car'</t>
+          <t>used car</t>
         </is>
       </c>
       <c r="D226" t="n">
@@ -10426,7 +10426,7 @@
       </c>
       <c r="C233" t="inlineStr">
         <is>
-          <t>'new car'</t>
+          <t>new car</t>
         </is>
       </c>
       <c r="D233" t="n">
@@ -10641,7 +10641,7 @@
       </c>
       <c r="C238" t="inlineStr">
         <is>
-          <t>'new car'</t>
+          <t>new car</t>
         </is>
       </c>
       <c r="D238" t="n">
@@ -10813,7 +10813,7 @@
       </c>
       <c r="C242" t="inlineStr">
         <is>
-          <t>'new car'</t>
+          <t>new car</t>
         </is>
       </c>
       <c r="D242" t="n">
@@ -10899,7 +10899,7 @@
       </c>
       <c r="C244" t="inlineStr">
         <is>
-          <t>'used car'</t>
+          <t>used car</t>
         </is>
       </c>
       <c r="D244" t="n">
@@ -11114,7 +11114,7 @@
       </c>
       <c r="C249" t="inlineStr">
         <is>
-          <t>'new car'</t>
+          <t>new car</t>
         </is>
       </c>
       <c r="D249" t="n">
@@ -11243,7 +11243,7 @@
       </c>
       <c r="C252" t="inlineStr">
         <is>
-          <t>'new car'</t>
+          <t>new car</t>
         </is>
       </c>
       <c r="D252" t="n">
@@ -11329,7 +11329,7 @@
       </c>
       <c r="C254" t="inlineStr">
         <is>
-          <t>'new car'</t>
+          <t>new car</t>
         </is>
       </c>
       <c r="D254" t="n">
@@ -11587,7 +11587,7 @@
       </c>
       <c r="C260" t="inlineStr">
         <is>
-          <t>'used car'</t>
+          <t>used car</t>
         </is>
       </c>
       <c r="D260" t="n">
@@ -11759,7 +11759,7 @@
       </c>
       <c r="C264" t="inlineStr">
         <is>
-          <t>'new car'</t>
+          <t>new car</t>
         </is>
       </c>
       <c r="D264" t="n">
@@ -11845,7 +11845,7 @@
       </c>
       <c r="C266" t="inlineStr">
         <is>
-          <t>'new car'</t>
+          <t>new car</t>
         </is>
       </c>
       <c r="D266" t="n">
@@ -12017,7 +12017,7 @@
       </c>
       <c r="C270" t="inlineStr">
         <is>
-          <t>'new car'</t>
+          <t>new car</t>
         </is>
       </c>
       <c r="D270" t="n">
@@ -12103,7 +12103,7 @@
       </c>
       <c r="C272" t="inlineStr">
         <is>
-          <t>'new car'</t>
+          <t>new car</t>
         </is>
       </c>
       <c r="D272" t="n">
@@ -12189,7 +12189,7 @@
       </c>
       <c r="C274" t="inlineStr">
         <is>
-          <t>'new car'</t>
+          <t>new car</t>
         </is>
       </c>
       <c r="D274" t="n">
@@ -12533,7 +12533,7 @@
       </c>
       <c r="C282" t="inlineStr">
         <is>
-          <t>'used car'</t>
+          <t>used car</t>
         </is>
       </c>
       <c r="D282" t="n">
@@ -12705,7 +12705,7 @@
       </c>
       <c r="C286" t="inlineStr">
         <is>
-          <t>'new car'</t>
+          <t>new car</t>
         </is>
       </c>
       <c r="D286" t="n">
@@ -12748,7 +12748,7 @@
       </c>
       <c r="C287" t="inlineStr">
         <is>
-          <t>'new car'</t>
+          <t>new car</t>
         </is>
       </c>
       <c r="D287" t="n">
@@ -12791,7 +12791,7 @@
       </c>
       <c r="C288" t="inlineStr">
         <is>
-          <t>'used car'</t>
+          <t>used car</t>
         </is>
       </c>
       <c r="D288" t="n">
@@ -13006,7 +13006,7 @@
       </c>
       <c r="C293" t="inlineStr">
         <is>
-          <t>'used car'</t>
+          <t>used car</t>
         </is>
       </c>
       <c r="D293" t="n">
@@ -13049,7 +13049,7 @@
       </c>
       <c r="C294" t="inlineStr">
         <is>
-          <t>'used car'</t>
+          <t>used car</t>
         </is>
       </c>
       <c r="D294" t="n">
@@ -13092,7 +13092,7 @@
       </c>
       <c r="C295" t="inlineStr">
         <is>
-          <t>'used car'</t>
+          <t>used car</t>
         </is>
       </c>
       <c r="D295" t="n">
@@ -13221,7 +13221,7 @@
       </c>
       <c r="C298" t="inlineStr">
         <is>
-          <t>'used car'</t>
+          <t>used car</t>
         </is>
       </c>
       <c r="D298" t="n">
@@ -13264,7 +13264,7 @@
       </c>
       <c r="C299" t="inlineStr">
         <is>
-          <t>'new car'</t>
+          <t>new car</t>
         </is>
       </c>
       <c r="D299" t="n">
@@ -13393,7 +13393,7 @@
       </c>
       <c r="C302" t="inlineStr">
         <is>
-          <t>'new car'</t>
+          <t>new car</t>
         </is>
       </c>
       <c r="D302" t="n">
@@ -13479,7 +13479,7 @@
       </c>
       <c r="C304" t="inlineStr">
         <is>
-          <t>'new car'</t>
+          <t>new car</t>
         </is>
       </c>
       <c r="D304" t="n">
@@ -13522,7 +13522,7 @@
       </c>
       <c r="C305" t="inlineStr">
         <is>
-          <t>'new car'</t>
+          <t>new car</t>
         </is>
       </c>
       <c r="D305" t="n">
@@ -13565,7 +13565,7 @@
       </c>
       <c r="C306" t="inlineStr">
         <is>
-          <t>'new car'</t>
+          <t>new car</t>
         </is>
       </c>
       <c r="D306" t="n">
@@ -13651,7 +13651,7 @@
       </c>
       <c r="C308" t="inlineStr">
         <is>
-          <t>'used car'</t>
+          <t>used car</t>
         </is>
       </c>
       <c r="D308" t="n">
@@ -13780,7 +13780,7 @@
       </c>
       <c r="C311" t="inlineStr">
         <is>
-          <t>'new car'</t>
+          <t>new car</t>
         </is>
       </c>
       <c r="D311" t="n">
@@ -13952,7 +13952,7 @@
       </c>
       <c r="C315" t="inlineStr">
         <is>
-          <t>'new car'</t>
+          <t>new car</t>
         </is>
       </c>
       <c r="D315" t="n">
@@ -13995,7 +13995,7 @@
       </c>
       <c r="C316" t="inlineStr">
         <is>
-          <t>'new car'</t>
+          <t>new car</t>
         </is>
       </c>
       <c r="D316" t="n">
@@ -14253,7 +14253,7 @@
       </c>
       <c r="C322" t="inlineStr">
         <is>
-          <t>'new car'</t>
+          <t>new car</t>
         </is>
       </c>
       <c r="D322" t="n">
@@ -14339,7 +14339,7 @@
       </c>
       <c r="C324" t="inlineStr">
         <is>
-          <t>'used car'</t>
+          <t>used car</t>
         </is>
       </c>
       <c r="D324" t="n">
@@ -14425,7 +14425,7 @@
       </c>
       <c r="C326" t="inlineStr">
         <is>
-          <t>'new car'</t>
+          <t>new car</t>
         </is>
       </c>
       <c r="D326" t="n">
@@ -14468,7 +14468,7 @@
       </c>
       <c r="C327" t="inlineStr">
         <is>
-          <t>'new car'</t>
+          <t>new car</t>
         </is>
       </c>
       <c r="D327" t="n">
@@ -14554,7 +14554,7 @@
       </c>
       <c r="C329" t="inlineStr">
         <is>
-          <t>'new car'</t>
+          <t>new car</t>
         </is>
       </c>
       <c r="D329" t="n">
@@ -14683,7 +14683,7 @@
       </c>
       <c r="C332" t="inlineStr">
         <is>
-          <t>'used car'</t>
+          <t>used car</t>
         </is>
       </c>
       <c r="D332" t="n">
@@ -14769,7 +14769,7 @@
       </c>
       <c r="C334" t="inlineStr">
         <is>
-          <t>'new car'</t>
+          <t>new car</t>
         </is>
       </c>
       <c r="D334" t="n">
@@ -14812,7 +14812,7 @@
       </c>
       <c r="C335" t="inlineStr">
         <is>
-          <t>'used car'</t>
+          <t>used car</t>
         </is>
       </c>
       <c r="D335" t="n">
@@ -14984,7 +14984,7 @@
       </c>
       <c r="C339" t="inlineStr">
         <is>
-          <t>'domestic appliance'</t>
+          <t>domestic appliance</t>
         </is>
       </c>
       <c r="D339" t="n">
@@ -15285,7 +15285,7 @@
       </c>
       <c r="C346" t="inlineStr">
         <is>
-          <t>'new car'</t>
+          <t>new car</t>
         </is>
       </c>
       <c r="D346" t="n">
@@ -15543,7 +15543,7 @@
       </c>
       <c r="C352" t="inlineStr">
         <is>
-          <t>'domestic appliance'</t>
+          <t>domestic appliance</t>
         </is>
       </c>
       <c r="D352" t="n">
@@ -15629,7 +15629,7 @@
       </c>
       <c r="C354" t="inlineStr">
         <is>
-          <t>'used car'</t>
+          <t>used car</t>
         </is>
       </c>
       <c r="D354" t="n">
@@ -15758,7 +15758,7 @@
       </c>
       <c r="C357" t="inlineStr">
         <is>
-          <t>'new car'</t>
+          <t>new car</t>
         </is>
       </c>
       <c r="D357" t="n">
@@ -16059,7 +16059,7 @@
       </c>
       <c r="C364" t="inlineStr">
         <is>
-          <t>'new car'</t>
+          <t>new car</t>
         </is>
       </c>
       <c r="D364" t="n">
@@ -16231,7 +16231,7 @@
       </c>
       <c r="C368" t="inlineStr">
         <is>
-          <t>'used car'</t>
+          <t>used car</t>
         </is>
       </c>
       <c r="D368" t="n">
@@ -16403,7 +16403,7 @@
       </c>
       <c r="C372" t="inlineStr">
         <is>
-          <t>'new car'</t>
+          <t>new car</t>
         </is>
       </c>
       <c r="D372" t="n">
@@ -16532,7 +16532,7 @@
       </c>
       <c r="C375" t="inlineStr">
         <is>
-          <t>'new car'</t>
+          <t>new car</t>
         </is>
       </c>
       <c r="D375" t="n">
@@ -16575,7 +16575,7 @@
       </c>
       <c r="C376" t="inlineStr">
         <is>
-          <t>the</t>
+          <t>other</t>
         </is>
       </c>
       <c r="D376" t="n">
@@ -16747,7 +16747,7 @@
       </c>
       <c r="C380" t="inlineStr">
         <is>
-          <t>'new car'</t>
+          <t>new car</t>
         </is>
       </c>
       <c r="D380" t="n">
@@ -16790,7 +16790,7 @@
       </c>
       <c r="C381" t="inlineStr">
         <is>
-          <t>'new car'</t>
+          <t>new car</t>
         </is>
       </c>
       <c r="D381" t="n">
@@ -16876,7 +16876,7 @@
       </c>
       <c r="C383" t="inlineStr">
         <is>
-          <t>'used car'</t>
+          <t>used car</t>
         </is>
       </c>
       <c r="D383" t="n">
@@ -16919,7 +16919,7 @@
       </c>
       <c r="C384" t="inlineStr">
         <is>
-          <t>'new car'</t>
+          <t>new car</t>
         </is>
       </c>
       <c r="D384" t="n">
@@ -16962,7 +16962,7 @@
       </c>
       <c r="C385" t="inlineStr">
         <is>
-          <t>'new car'</t>
+          <t>new car</t>
         </is>
       </c>
       <c r="D385" t="n">
@@ -17263,7 +17263,7 @@
       </c>
       <c r="C392" t="inlineStr">
         <is>
-          <t>'new car'</t>
+          <t>new car</t>
         </is>
       </c>
       <c r="D392" t="n">
@@ -17349,7 +17349,7 @@
       </c>
       <c r="C394" t="inlineStr">
         <is>
-          <t>'new car'</t>
+          <t>new car</t>
         </is>
       </c>
       <c r="D394" t="n">
@@ -17607,7 +17607,7 @@
       </c>
       <c r="C400" t="inlineStr">
         <is>
-          <t>'new car'</t>
+          <t>new car</t>
         </is>
       </c>
       <c r="D400" t="n">
@@ -17822,7 +17822,7 @@
       </c>
       <c r="C405" t="inlineStr">
         <is>
-          <t>'new car'</t>
+          <t>new car</t>
         </is>
       </c>
       <c r="D405" t="n">
@@ -17865,7 +17865,7 @@
       </c>
       <c r="C406" t="inlineStr">
         <is>
-          <t>'new car'</t>
+          <t>new car</t>
         </is>
       </c>
       <c r="D406" t="n">
@@ -17951,7 +17951,7 @@
       </c>
       <c r="C408" t="inlineStr">
         <is>
-          <t>'used car'</t>
+          <t>used car</t>
         </is>
       </c>
       <c r="D408" t="n">
@@ -18080,7 +18080,7 @@
       </c>
       <c r="C411" t="inlineStr">
         <is>
-          <t>'new car'</t>
+          <t>new car</t>
         </is>
       </c>
       <c r="D411" t="n">
@@ -18166,7 +18166,7 @@
       </c>
       <c r="C413" t="inlineStr">
         <is>
-          <t>'used car'</t>
+          <t>used car</t>
         </is>
       </c>
       <c r="D413" t="n">
@@ -18252,7 +18252,7 @@
       </c>
       <c r="C415" t="inlineStr">
         <is>
-          <t>'new car'</t>
+          <t>new car</t>
         </is>
       </c>
       <c r="D415" t="n">
@@ -18295,7 +18295,7 @@
       </c>
       <c r="C416" t="inlineStr">
         <is>
-          <t>'new car'</t>
+          <t>new car</t>
         </is>
       </c>
       <c r="D416" t="n">
@@ -18338,7 +18338,7 @@
       </c>
       <c r="C417" t="inlineStr">
         <is>
-          <t>'used car'</t>
+          <t>used car</t>
         </is>
       </c>
       <c r="D417" t="n">
@@ -18381,7 +18381,7 @@
       </c>
       <c r="C418" t="inlineStr">
         <is>
-          <t>'new car'</t>
+          <t>new car</t>
         </is>
       </c>
       <c r="D418" t="n">
@@ -18402,7 +18402,7 @@
       </c>
       <c r="H418" t="inlineStr">
         <is>
-          <t>unskilled resident</t>
+          <t>'unskilled resident'</t>
         </is>
       </c>
       <c r="I418" t="inlineStr">
@@ -18467,7 +18467,7 @@
       </c>
       <c r="C420" t="inlineStr">
         <is>
-          <t>'new car'</t>
+          <t>new car</t>
         </is>
       </c>
       <c r="D420" t="n">
@@ -18510,7 +18510,7 @@
       </c>
       <c r="C421" t="inlineStr">
         <is>
-          <t>'new car'</t>
+          <t>new car</t>
         </is>
       </c>
       <c r="D421" t="n">
@@ -18553,7 +18553,7 @@
       </c>
       <c r="C422" t="inlineStr">
         <is>
-          <t>'new car'</t>
+          <t>new car</t>
         </is>
       </c>
       <c r="D422" t="n">
@@ -18596,7 +18596,7 @@
       </c>
       <c r="C423" t="inlineStr">
         <is>
-          <t>'used car'</t>
+          <t>used car</t>
         </is>
       </c>
       <c r="D423" t="n">
@@ -18639,7 +18639,7 @@
       </c>
       <c r="C424" t="inlineStr">
         <is>
-          <t>'new car'</t>
+          <t>new car</t>
         </is>
       </c>
       <c r="D424" t="n">
@@ -18768,7 +18768,7 @@
       </c>
       <c r="C427" t="inlineStr">
         <is>
-          <t>'used car'</t>
+          <t>used car</t>
         </is>
       </c>
       <c r="D427" t="n">
@@ -19284,7 +19284,7 @@
       </c>
       <c r="C439" t="inlineStr">
         <is>
-          <t>'new car'</t>
+          <t>new car</t>
         </is>
       </c>
       <c r="D439" t="n">
@@ -19413,7 +19413,7 @@
       </c>
       <c r="C442" t="inlineStr">
         <is>
-          <t>'new car'</t>
+          <t>new car</t>
         </is>
       </c>
       <c r="D442" t="n">
@@ -19671,7 +19671,7 @@
       </c>
       <c r="C448" t="inlineStr">
         <is>
-          <t>'new car'</t>
+          <t>new car</t>
         </is>
       </c>
       <c r="D448" t="n">
@@ -19843,7 +19843,7 @@
       </c>
       <c r="C452" t="inlineStr">
         <is>
-          <t>'used car'</t>
+          <t>used car</t>
         </is>
       </c>
       <c r="D452" t="n">
@@ -19972,7 +19972,7 @@
       </c>
       <c r="C455" t="inlineStr">
         <is>
-          <t>'used car'</t>
+          <t>used car</t>
         </is>
       </c>
       <c r="D455" t="n">
@@ -20015,7 +20015,7 @@
       </c>
       <c r="C456" t="inlineStr">
         <is>
-          <t>'new car'</t>
+          <t>new car</t>
         </is>
       </c>
       <c r="D456" t="n">
@@ -20058,7 +20058,7 @@
       </c>
       <c r="C457" t="inlineStr">
         <is>
-          <t>'used car'</t>
+          <t>used car</t>
         </is>
       </c>
       <c r="D457" t="n">
@@ -20101,7 +20101,7 @@
       </c>
       <c r="C458" t="inlineStr">
         <is>
-          <t>'new car'</t>
+          <t>new car</t>
         </is>
       </c>
       <c r="D458" t="n">
@@ -20144,7 +20144,7 @@
       </c>
       <c r="C459" t="inlineStr">
         <is>
-          <t>'used car'</t>
+          <t>used car</t>
         </is>
       </c>
       <c r="D459" t="n">
@@ -20187,7 +20187,7 @@
       </c>
       <c r="C460" t="inlineStr">
         <is>
-          <t>'domestic appliance'</t>
+          <t>domestic appliance</t>
         </is>
       </c>
       <c r="D460" t="n">
@@ -20316,7 +20316,7 @@
       </c>
       <c r="C463" t="inlineStr">
         <is>
-          <t>'new car'</t>
+          <t>new car</t>
         </is>
       </c>
       <c r="D463" t="n">
@@ -20488,7 +20488,7 @@
       </c>
       <c r="C467" t="inlineStr">
         <is>
-          <t>'used car'</t>
+          <t>used car</t>
         </is>
       </c>
       <c r="D467" t="n">
@@ -20660,7 +20660,7 @@
       </c>
       <c r="C471" t="inlineStr">
         <is>
-          <t>'used car'</t>
+          <t>used car</t>
         </is>
       </c>
       <c r="D471" t="n">
@@ -20789,7 +20789,7 @@
       </c>
       <c r="C474" t="inlineStr">
         <is>
-          <t>'new car'</t>
+          <t>new car</t>
         </is>
       </c>
       <c r="D474" t="n">
@@ -20961,7 +20961,7 @@
       </c>
       <c r="C478" t="inlineStr">
         <is>
-          <t>'used car'</t>
+          <t>used car</t>
         </is>
       </c>
       <c r="D478" t="n">
@@ -21176,7 +21176,7 @@
       </c>
       <c r="C483" t="inlineStr">
         <is>
-          <t>'new car'</t>
+          <t>new car</t>
         </is>
       </c>
       <c r="D483" t="n">
@@ -21305,7 +21305,7 @@
       </c>
       <c r="C486" t="inlineStr">
         <is>
-          <t>'new car'</t>
+          <t>new car</t>
         </is>
       </c>
       <c r="D486" t="n">
@@ -21348,7 +21348,7 @@
       </c>
       <c r="C487" t="inlineStr">
         <is>
-          <t>'new car'</t>
+          <t>new car</t>
         </is>
       </c>
       <c r="D487" t="n">
@@ -21434,7 +21434,7 @@
       </c>
       <c r="C489" t="inlineStr">
         <is>
-          <t>'new car'</t>
+          <t>new car</t>
         </is>
       </c>
       <c r="D489" t="n">
@@ -21477,7 +21477,7 @@
       </c>
       <c r="C490" t="inlineStr">
         <is>
-          <t>'new car'</t>
+          <t>new car</t>
         </is>
       </c>
       <c r="D490" t="n">
@@ -21520,7 +21520,7 @@
       </c>
       <c r="C491" t="inlineStr">
         <is>
-          <t>'new car'</t>
+          <t>new car</t>
         </is>
       </c>
       <c r="D491" t="n">
@@ -21735,7 +21735,7 @@
       </c>
       <c r="C496" t="inlineStr">
         <is>
-          <t>'new car'</t>
+          <t>new car</t>
         </is>
       </c>
       <c r="D496" t="n">
@@ -21950,7 +21950,7 @@
       </c>
       <c r="C501" t="inlineStr">
         <is>
-          <t>'new car'</t>
+          <t>new car</t>
         </is>
       </c>
       <c r="D501" t="n">
@@ -21993,7 +21993,7 @@
       </c>
       <c r="C502" t="inlineStr">
         <is>
-          <t>'new car'</t>
+          <t>new car</t>
         </is>
       </c>
       <c r="D502" t="n">
@@ -22036,7 +22036,7 @@
       </c>
       <c r="C503" t="inlineStr">
         <is>
-          <t>'used car'</t>
+          <t>used car</t>
         </is>
       </c>
       <c r="D503" t="n">
@@ -22165,7 +22165,7 @@
       </c>
       <c r="C506" t="inlineStr">
         <is>
-          <t>'new car'</t>
+          <t>new car</t>
         </is>
       </c>
       <c r="D506" t="n">
@@ -22208,7 +22208,7 @@
       </c>
       <c r="C507" t="inlineStr">
         <is>
-          <t>'new car'</t>
+          <t>new car</t>
         </is>
       </c>
       <c r="D507" t="n">
@@ -22251,7 +22251,7 @@
       </c>
       <c r="C508" t="inlineStr">
         <is>
-          <t>'used car'</t>
+          <t>used car</t>
         </is>
       </c>
       <c r="D508" t="n">
@@ -22294,7 +22294,7 @@
       </c>
       <c r="C509" t="inlineStr">
         <is>
-          <t>'new car'</t>
+          <t>new car</t>
         </is>
       </c>
       <c r="D509" t="n">
@@ -22380,7 +22380,7 @@
       </c>
       <c r="C511" t="inlineStr">
         <is>
-          <t>'used car'</t>
+          <t>used car</t>
         </is>
       </c>
       <c r="D511" t="n">
@@ -22423,7 +22423,7 @@
       </c>
       <c r="C512" t="inlineStr">
         <is>
-          <t>'new car'</t>
+          <t>new car</t>
         </is>
       </c>
       <c r="D512" t="n">
@@ -22466,7 +22466,7 @@
       </c>
       <c r="C513" t="inlineStr">
         <is>
-          <t>'used car'</t>
+          <t>used car</t>
         </is>
       </c>
       <c r="D513" t="n">
@@ -22595,7 +22595,7 @@
       </c>
       <c r="C516" t="inlineStr">
         <is>
-          <t>'new car'</t>
+          <t>new car</t>
         </is>
       </c>
       <c r="D516" t="n">
@@ -22638,7 +22638,7 @@
       </c>
       <c r="C517" t="inlineStr">
         <is>
-          <t>'new car'</t>
+          <t>new car</t>
         </is>
       </c>
       <c r="D517" t="n">
@@ -22681,7 +22681,7 @@
       </c>
       <c r="C518" t="inlineStr">
         <is>
-          <t>'new car'</t>
+          <t>new car</t>
         </is>
       </c>
       <c r="D518" t="n">
@@ -22767,7 +22767,7 @@
       </c>
       <c r="C520" t="inlineStr">
         <is>
-          <t>'new car'</t>
+          <t>new car</t>
         </is>
       </c>
       <c r="D520" t="n">
@@ -22982,7 +22982,7 @@
       </c>
       <c r="C525" t="inlineStr">
         <is>
-          <t>'used car'</t>
+          <t>used car</t>
         </is>
       </c>
       <c r="D525" t="n">
@@ -23068,7 +23068,7 @@
       </c>
       <c r="C527" t="inlineStr">
         <is>
-          <t>'used car'</t>
+          <t>used car</t>
         </is>
       </c>
       <c r="D527" t="n">
@@ -23240,7 +23240,7 @@
       </c>
       <c r="C531" t="inlineStr">
         <is>
-          <t>'new car'</t>
+          <t>new car</t>
         </is>
       </c>
       <c r="D531" t="n">
@@ -23326,7 +23326,7 @@
       </c>
       <c r="C533" t="inlineStr">
         <is>
-          <t>'new car'</t>
+          <t>new car</t>
         </is>
       </c>
       <c r="D533" t="n">
@@ -23369,7 +23369,7 @@
       </c>
       <c r="C534" t="inlineStr">
         <is>
-          <t>'used car'</t>
+          <t>used car</t>
         </is>
       </c>
       <c r="D534" t="n">
@@ -23541,7 +23541,7 @@
       </c>
       <c r="C538" t="inlineStr">
         <is>
-          <t>'new car'</t>
+          <t>new car</t>
         </is>
       </c>
       <c r="D538" t="n">
@@ -23627,7 +23627,7 @@
       </c>
       <c r="C540" t="inlineStr">
         <is>
-          <t>'new car'</t>
+          <t>new car</t>
         </is>
       </c>
       <c r="D540" t="n">
@@ -23756,7 +23756,7 @@
       </c>
       <c r="C543" t="inlineStr">
         <is>
-          <t>'new car'</t>
+          <t>new car</t>
         </is>
       </c>
       <c r="D543" t="n">
@@ -23885,7 +23885,7 @@
       </c>
       <c r="C546" t="inlineStr">
         <is>
-          <t>'new car'</t>
+          <t>new car</t>
         </is>
       </c>
       <c r="D546" t="n">
@@ -23928,7 +23928,7 @@
       </c>
       <c r="C547" t="inlineStr">
         <is>
-          <t>'new car'</t>
+          <t>new car</t>
         </is>
       </c>
       <c r="D547" t="n">
@@ -23971,7 +23971,7 @@
       </c>
       <c r="C548" t="inlineStr">
         <is>
-          <t>'new car'</t>
+          <t>new car</t>
         </is>
       </c>
       <c r="D548" t="n">
@@ -24100,7 +24100,7 @@
       </c>
       <c r="C551" t="inlineStr">
         <is>
-          <t>'used car'</t>
+          <t>used car</t>
         </is>
       </c>
       <c r="D551" t="n">
@@ -24272,7 +24272,7 @@
       </c>
       <c r="C555" t="inlineStr">
         <is>
-          <t>'new car'</t>
+          <t>new car</t>
         </is>
       </c>
       <c r="D555" t="n">
@@ -24401,7 +24401,7 @@
       </c>
       <c r="C558" t="inlineStr">
         <is>
-          <t>'new car'</t>
+          <t>new car</t>
         </is>
       </c>
       <c r="D558" t="n">
@@ -24444,7 +24444,7 @@
       </c>
       <c r="C559" t="inlineStr">
         <is>
-          <t>'new car'</t>
+          <t>new car</t>
         </is>
       </c>
       <c r="D559" t="n">
@@ -24573,7 +24573,7 @@
       </c>
       <c r="C562" t="inlineStr">
         <is>
-          <t>'used car'</t>
+          <t>used car</t>
         </is>
       </c>
       <c r="D562" t="n">
@@ -24702,7 +24702,7 @@
       </c>
       <c r="C565" t="inlineStr">
         <is>
-          <t>'new car'</t>
+          <t>new car</t>
         </is>
       </c>
       <c r="D565" t="n">
@@ -24831,7 +24831,7 @@
       </c>
       <c r="C568" t="inlineStr">
         <is>
-          <t>'new car'</t>
+          <t>new car</t>
         </is>
       </c>
       <c r="D568" t="n">
@@ -25089,7 +25089,7 @@
       </c>
       <c r="C574" t="inlineStr">
         <is>
-          <t>'used car'</t>
+          <t>used car</t>
         </is>
       </c>
       <c r="D574" t="n">
@@ -25347,7 +25347,7 @@
       </c>
       <c r="C580" t="inlineStr">
         <is>
-          <t>'new car'</t>
+          <t>new car</t>
         </is>
       </c>
       <c r="D580" t="n">
@@ -25433,7 +25433,7 @@
       </c>
       <c r="C582" t="inlineStr">
         <is>
-          <t>'new car'</t>
+          <t>new car</t>
         </is>
       </c>
       <c r="D582" t="n">
@@ -25476,7 +25476,7 @@
       </c>
       <c r="C583" t="inlineStr">
         <is>
-          <t>'new car'</t>
+          <t>new car</t>
         </is>
       </c>
       <c r="D583" t="n">
@@ -25605,7 +25605,7 @@
       </c>
       <c r="C586" t="inlineStr">
         <is>
-          <t>'new car'</t>
+          <t>new car</t>
         </is>
       </c>
       <c r="D586" t="n">
@@ -25691,7 +25691,7 @@
       </c>
       <c r="C588" t="inlineStr">
         <is>
-          <t>'new car'</t>
+          <t>new car</t>
         </is>
       </c>
       <c r="D588" t="n">
@@ -25777,7 +25777,7 @@
       </c>
       <c r="C590" t="inlineStr">
         <is>
-          <t>'domestic appliance'</t>
+          <t>domestic appliance</t>
         </is>
       </c>
       <c r="D590" t="n">
@@ -25906,7 +25906,7 @@
       </c>
       <c r="C593" t="inlineStr">
         <is>
-          <t>'new car'</t>
+          <t>new car</t>
         </is>
       </c>
       <c r="D593" t="n">
@@ -25992,7 +25992,7 @@
       </c>
       <c r="C595" t="inlineStr">
         <is>
-          <t>'new car'</t>
+          <t>new car</t>
         </is>
       </c>
       <c r="D595" t="n">
@@ -26078,7 +26078,7 @@
       </c>
       <c r="C597" t="inlineStr">
         <is>
-          <t>'new car'</t>
+          <t>new car</t>
         </is>
       </c>
       <c r="D597" t="n">
@@ -26121,7 +26121,7 @@
       </c>
       <c r="C598" t="inlineStr">
         <is>
-          <t>'new car'</t>
+          <t>new car</t>
         </is>
       </c>
       <c r="D598" t="n">
@@ -26207,7 +26207,7 @@
       </c>
       <c r="C600" t="inlineStr">
         <is>
-          <t>'new car'</t>
+          <t>new car</t>
         </is>
       </c>
       <c r="D600" t="n">
@@ -26680,7 +26680,7 @@
       </c>
       <c r="C611" t="inlineStr">
         <is>
-          <t>'used car'</t>
+          <t>used car</t>
         </is>
       </c>
       <c r="D611" t="n">
@@ -26723,7 +26723,7 @@
       </c>
       <c r="C612" t="inlineStr">
         <is>
-          <t>'domestic appliance'</t>
+          <t>domestic appliance</t>
         </is>
       </c>
       <c r="D612" t="n">
@@ -26766,7 +26766,7 @@
       </c>
       <c r="C613" t="inlineStr">
         <is>
-          <t>'new car'</t>
+          <t>new car</t>
         </is>
       </c>
       <c r="D613" t="n">
@@ -26852,7 +26852,7 @@
       </c>
       <c r="C615" t="inlineStr">
         <is>
-          <t>'used car'</t>
+          <t>used car</t>
         </is>
       </c>
       <c r="D615" t="n">
@@ -27024,7 +27024,7 @@
       </c>
       <c r="C619" t="inlineStr">
         <is>
-          <t>'new car'</t>
+          <t>new car</t>
         </is>
       </c>
       <c r="D619" t="n">
@@ -27110,7 +27110,7 @@
       </c>
       <c r="C621" t="inlineStr">
         <is>
-          <t>'new car'</t>
+          <t>new car</t>
         </is>
       </c>
       <c r="D621" t="n">
@@ -27196,7 +27196,7 @@
       </c>
       <c r="C623" t="inlineStr">
         <is>
-          <t>'new car'</t>
+          <t>new car</t>
         </is>
       </c>
       <c r="D623" t="n">
@@ -27454,7 +27454,7 @@
       </c>
       <c r="C629" t="inlineStr">
         <is>
-          <t>'new car'</t>
+          <t>new car</t>
         </is>
       </c>
       <c r="D629" t="n">
@@ -27755,7 +27755,7 @@
       </c>
       <c r="C636" t="inlineStr">
         <is>
-          <t>'new car'</t>
+          <t>new car</t>
         </is>
       </c>
       <c r="D636" t="n">
@@ -28314,7 +28314,7 @@
       </c>
       <c r="C649" t="inlineStr">
         <is>
-          <t>'new car'</t>
+          <t>new car</t>
         </is>
       </c>
       <c r="D649" t="n">
@@ -28357,7 +28357,7 @@
       </c>
       <c r="C650" t="inlineStr">
         <is>
-          <t>'new car'</t>
+          <t>new car</t>
         </is>
       </c>
       <c r="D650" t="n">
@@ -28529,7 +28529,7 @@
       </c>
       <c r="C654" t="inlineStr">
         <is>
-          <t>'new car'</t>
+          <t>new car</t>
         </is>
       </c>
       <c r="D654" t="n">
@@ -28572,7 +28572,7 @@
       </c>
       <c r="C655" t="inlineStr">
         <is>
-          <t>'new car'</t>
+          <t>new car</t>
         </is>
       </c>
       <c r="D655" t="n">
@@ -28615,7 +28615,7 @@
       </c>
       <c r="C656" t="inlineStr">
         <is>
-          <t>'used car'</t>
+          <t>used car</t>
         </is>
       </c>
       <c r="D656" t="n">
@@ -28658,7 +28658,7 @@
       </c>
       <c r="C657" t="inlineStr">
         <is>
-          <t>'new car'</t>
+          <t>new car</t>
         </is>
       </c>
       <c r="D657" t="n">
@@ -28701,7 +28701,7 @@
       </c>
       <c r="C658" t="inlineStr">
         <is>
-          <t>'new car'</t>
+          <t>new car</t>
         </is>
       </c>
       <c r="D658" t="n">
@@ -28916,7 +28916,7 @@
       </c>
       <c r="C663" t="inlineStr">
         <is>
-          <t>'new car'</t>
+          <t>new car</t>
         </is>
       </c>
       <c r="D663" t="n">
@@ -29217,7 +29217,7 @@
       </c>
       <c r="C670" t="inlineStr">
         <is>
-          <t>'new car'</t>
+          <t>new car</t>
         </is>
       </c>
       <c r="D670" t="n">
@@ -29389,7 +29389,7 @@
       </c>
       <c r="C674" t="inlineStr">
         <is>
-          <t>'new car'</t>
+          <t>new car</t>
         </is>
       </c>
       <c r="D674" t="n">
@@ -29432,7 +29432,7 @@
       </c>
       <c r="C675" t="inlineStr">
         <is>
-          <t>'new car'</t>
+          <t>new car</t>
         </is>
       </c>
       <c r="D675" t="n">
@@ -29948,7 +29948,7 @@
       </c>
       <c r="C687" t="inlineStr">
         <is>
-          <t>'new car'</t>
+          <t>new car</t>
         </is>
       </c>
       <c r="D687" t="n">
@@ -30034,7 +30034,7 @@
       </c>
       <c r="C689" t="inlineStr">
         <is>
-          <t>'new car'</t>
+          <t>new car</t>
         </is>
       </c>
       <c r="D689" t="n">
@@ -30120,7 +30120,7 @@
       </c>
       <c r="C691" t="inlineStr">
         <is>
-          <t>'new car'</t>
+          <t>new car</t>
         </is>
       </c>
       <c r="D691" t="n">
@@ -30292,7 +30292,7 @@
       </c>
       <c r="C695" t="inlineStr">
         <is>
-          <t>'new car'</t>
+          <t>new car</t>
         </is>
       </c>
       <c r="D695" t="n">
@@ -30378,7 +30378,7 @@
       </c>
       <c r="C697" t="inlineStr">
         <is>
-          <t>'used car'</t>
+          <t>used car</t>
         </is>
       </c>
       <c r="D697" t="n">
@@ -30464,7 +30464,7 @@
       </c>
       <c r="C699" t="inlineStr">
         <is>
-          <t>'new car'</t>
+          <t>new car</t>
         </is>
       </c>
       <c r="D699" t="n">
@@ -30636,7 +30636,7 @@
       </c>
       <c r="C703" t="inlineStr">
         <is>
-          <t>'used car'</t>
+          <t>used car</t>
         </is>
       </c>
       <c r="D703" t="n">
@@ -30808,7 +30808,7 @@
       </c>
       <c r="C707" t="inlineStr">
         <is>
-          <t>'new car'</t>
+          <t>new car</t>
         </is>
       </c>
       <c r="D707" t="n">
@@ -30851,7 +30851,7 @@
       </c>
       <c r="C708" t="inlineStr">
         <is>
-          <t>'new car'</t>
+          <t>new car</t>
         </is>
       </c>
       <c r="D708" t="n">
@@ -31109,7 +31109,7 @@
       </c>
       <c r="C714" t="inlineStr">
         <is>
-          <t>'used car'</t>
+          <t>used car</t>
         </is>
       </c>
       <c r="D714" t="n">
@@ -31195,7 +31195,7 @@
       </c>
       <c r="C716" t="inlineStr">
         <is>
-          <t>'new car'</t>
+          <t>new car</t>
         </is>
       </c>
       <c r="D716" t="n">
@@ -31238,7 +31238,7 @@
       </c>
       <c r="C717" t="inlineStr">
         <is>
-          <t>'used car'</t>
+          <t>used car</t>
         </is>
       </c>
       <c r="D717" t="n">
@@ -31410,7 +31410,7 @@
       </c>
       <c r="C721" t="inlineStr">
         <is>
-          <t>'used car'</t>
+          <t>used car</t>
         </is>
       </c>
       <c r="D721" t="n">
@@ -31539,7 +31539,7 @@
       </c>
       <c r="C724" t="inlineStr">
         <is>
-          <t>'new car'</t>
+          <t>new car</t>
         </is>
       </c>
       <c r="D724" t="n">
@@ -31625,7 +31625,7 @@
       </c>
       <c r="C726" t="inlineStr">
         <is>
-          <t>'new car'</t>
+          <t>new car</t>
         </is>
       </c>
       <c r="D726" t="n">
@@ -31668,7 +31668,7 @@
       </c>
       <c r="C727" t="inlineStr">
         <is>
-          <t>'new car'</t>
+          <t>new car</t>
         </is>
       </c>
       <c r="D727" t="n">
@@ -31947,7 +31947,7 @@
       </c>
       <c r="H733" t="inlineStr">
         <is>
-          <t>unskilled resident</t>
+          <t>'unskilled resident'</t>
         </is>
       </c>
       <c r="I733" t="inlineStr">
@@ -32012,7 +32012,7 @@
       </c>
       <c r="C735" t="inlineStr">
         <is>
-          <t>'used car'</t>
+          <t>used car</t>
         </is>
       </c>
       <c r="D735" t="n">
@@ -32055,7 +32055,7 @@
       </c>
       <c r="C736" t="inlineStr">
         <is>
-          <t>'new car'</t>
+          <t>new car</t>
         </is>
       </c>
       <c r="D736" t="n">
@@ -32098,7 +32098,7 @@
       </c>
       <c r="C737" t="inlineStr">
         <is>
-          <t>'domestic appliance'</t>
+          <t>domestic appliance</t>
         </is>
       </c>
       <c r="D737" t="n">
@@ -32141,7 +32141,7 @@
       </c>
       <c r="C738" t="inlineStr">
         <is>
-          <t>'used car'</t>
+          <t>used car</t>
         </is>
       </c>
       <c r="D738" t="n">
@@ -32184,7 +32184,7 @@
       </c>
       <c r="C739" t="inlineStr">
         <is>
-          <t>'new car'</t>
+          <t>new car</t>
         </is>
       </c>
       <c r="D739" t="n">
@@ -32227,7 +32227,7 @@
       </c>
       <c r="C740" t="inlineStr">
         <is>
-          <t>'new car'</t>
+          <t>new car</t>
         </is>
       </c>
       <c r="D740" t="n">
@@ -32313,7 +32313,7 @@
       </c>
       <c r="C742" t="inlineStr">
         <is>
-          <t>'new car'</t>
+          <t>new car</t>
         </is>
       </c>
       <c r="D742" t="n">
@@ -32571,7 +32571,7 @@
       </c>
       <c r="C748" t="inlineStr">
         <is>
-          <t>'new car'</t>
+          <t>new car</t>
         </is>
       </c>
       <c r="D748" t="n">
@@ -32614,7 +32614,7 @@
       </c>
       <c r="C749" t="inlineStr">
         <is>
-          <t>'new car'</t>
+          <t>new car</t>
         </is>
       </c>
       <c r="D749" t="n">
@@ -32657,7 +32657,7 @@
       </c>
       <c r="C750" t="inlineStr">
         <is>
-          <t>use car'</t>
+          <t>used car</t>
         </is>
       </c>
       <c r="D750" t="n">
@@ -32700,7 +32700,7 @@
       </c>
       <c r="C751" t="inlineStr">
         <is>
-          <t>'used car'</t>
+          <t>used car</t>
         </is>
       </c>
       <c r="D751" t="n">
@@ -32786,7 +32786,7 @@
       </c>
       <c r="C753" t="inlineStr">
         <is>
-          <t>'new car'</t>
+          <t>new car</t>
         </is>
       </c>
       <c r="D753" t="n">
@@ -32958,7 +32958,7 @@
       </c>
       <c r="C757" t="inlineStr">
         <is>
-          <t>'new car'</t>
+          <t>new car</t>
         </is>
       </c>
       <c r="D757" t="n">
@@ -33001,7 +33001,7 @@
       </c>
       <c r="C758" t="inlineStr">
         <is>
-          <t>'new car'</t>
+          <t>new car</t>
         </is>
       </c>
       <c r="D758" t="n">
@@ -33087,7 +33087,7 @@
       </c>
       <c r="C760" t="inlineStr">
         <is>
-          <t>'new car'</t>
+          <t>new car</t>
         </is>
       </c>
       <c r="D760" t="n">
@@ -33130,7 +33130,7 @@
       </c>
       <c r="C761" t="inlineStr">
         <is>
-          <t>'new car'</t>
+          <t>new car</t>
         </is>
       </c>
       <c r="D761" t="n">
@@ -33173,7 +33173,7 @@
       </c>
       <c r="C762" t="inlineStr">
         <is>
-          <t>'new car'</t>
+          <t>new car</t>
         </is>
       </c>
       <c r="D762" t="n">
@@ -33302,7 +33302,7 @@
       </c>
       <c r="C765" t="inlineStr">
         <is>
-          <t>'new car'</t>
+          <t>new car</t>
         </is>
       </c>
       <c r="D765" t="n">
@@ -33345,7 +33345,7 @@
       </c>
       <c r="C766" t="inlineStr">
         <is>
-          <t>'new car'</t>
+          <t>new car</t>
         </is>
       </c>
       <c r="D766" t="n">
@@ -33474,7 +33474,7 @@
       </c>
       <c r="C769" t="inlineStr">
         <is>
-          <t>'used car'</t>
+          <t>used car</t>
         </is>
       </c>
       <c r="D769" t="n">
@@ -33603,7 +33603,7 @@
       </c>
       <c r="C772" t="inlineStr">
         <is>
-          <t>'used car'</t>
+          <t>used car</t>
         </is>
       </c>
       <c r="D772" t="n">
@@ -33689,7 +33689,7 @@
       </c>
       <c r="C774" t="inlineStr">
         <is>
-          <t>'used car'</t>
+          <t>used car</t>
         </is>
       </c>
       <c r="D774" t="n">
@@ -33775,7 +33775,7 @@
       </c>
       <c r="C776" t="inlineStr">
         <is>
-          <t>'new car'</t>
+          <t>new car</t>
         </is>
       </c>
       <c r="D776" t="n">
@@ -33818,7 +33818,7 @@
       </c>
       <c r="C777" t="inlineStr">
         <is>
-          <t>'new car'</t>
+          <t>new car</t>
         </is>
       </c>
       <c r="D777" t="n">
@@ -33861,7 +33861,7 @@
       </c>
       <c r="C778" t="inlineStr">
         <is>
-          <t>'new car'</t>
+          <t>new car</t>
         </is>
       </c>
       <c r="D778" t="n">
@@ -33947,7 +33947,7 @@
       </c>
       <c r="C780" t="inlineStr">
         <is>
-          <t>'used car'</t>
+          <t>used car</t>
         </is>
       </c>
       <c r="D780" t="n">
@@ -34076,7 +34076,7 @@
       </c>
       <c r="C783" t="inlineStr">
         <is>
-          <t>'new car'</t>
+          <t>new car</t>
         </is>
       </c>
       <c r="D783" t="n">
@@ -34162,7 +34162,7 @@
       </c>
       <c r="C785" t="inlineStr">
         <is>
-          <t>'new car'</t>
+          <t>new car</t>
         </is>
       </c>
       <c r="D785" t="n">
@@ -34205,7 +34205,7 @@
       </c>
       <c r="C786" t="inlineStr">
         <is>
-          <t>'used car'</t>
+          <t>used car</t>
         </is>
       </c>
       <c r="D786" t="n">
@@ -34334,7 +34334,7 @@
       </c>
       <c r="C789" t="inlineStr">
         <is>
-          <t>'used car'</t>
+          <t>used car</t>
         </is>
       </c>
       <c r="D789" t="n">
@@ -34506,7 +34506,7 @@
       </c>
       <c r="C793" t="inlineStr">
         <is>
-          <t>'used car'</t>
+          <t>used car</t>
         </is>
       </c>
       <c r="D793" t="n">
@@ -34721,7 +34721,7 @@
       </c>
       <c r="C798" t="inlineStr">
         <is>
-          <t>'used car'</t>
+          <t>used car</t>
         </is>
       </c>
       <c r="D798" t="n">
@@ -34807,7 +34807,7 @@
       </c>
       <c r="C800" t="inlineStr">
         <is>
-          <t>'new car'</t>
+          <t>new car</t>
         </is>
       </c>
       <c r="D800" t="n">
@@ -34850,7 +34850,7 @@
       </c>
       <c r="C801" t="inlineStr">
         <is>
-          <t>'new car'</t>
+          <t>new car</t>
         </is>
       </c>
       <c r="D801" t="n">
@@ -35065,7 +35065,7 @@
       </c>
       <c r="C806" t="inlineStr">
         <is>
-          <t>'new car'</t>
+          <t>new car</t>
         </is>
       </c>
       <c r="D806" t="n">
@@ -35108,7 +35108,7 @@
       </c>
       <c r="C807" t="inlineStr">
         <is>
-          <t>'new car'</t>
+          <t>new car</t>
         </is>
       </c>
       <c r="D807" t="n">
@@ -35237,7 +35237,7 @@
       </c>
       <c r="C810" t="inlineStr">
         <is>
-          <t>'used car'</t>
+          <t>used car</t>
         </is>
       </c>
       <c r="D810" t="n">
@@ -35280,7 +35280,7 @@
       </c>
       <c r="C811" t="inlineStr">
         <is>
-          <t>'new car'</t>
+          <t>new car</t>
         </is>
       </c>
       <c r="D811" t="n">
@@ -35409,7 +35409,7 @@
       </c>
       <c r="C814" t="inlineStr">
         <is>
-          <t>'used car'</t>
+          <t>used car</t>
         </is>
       </c>
       <c r="D814" t="n">
@@ -35452,7 +35452,7 @@
       </c>
       <c r="C815" t="inlineStr">
         <is>
-          <t>'domestic appliance'</t>
+          <t>domestic appliance</t>
         </is>
       </c>
       <c r="D815" t="n">
@@ -35495,7 +35495,7 @@
       </c>
       <c r="C816" t="inlineStr">
         <is>
-          <t>'new car'</t>
+          <t>new car</t>
         </is>
       </c>
       <c r="D816" t="n">
@@ -35538,7 +35538,7 @@
       </c>
       <c r="C817" t="inlineStr">
         <is>
-          <t>'new car'</t>
+          <t>new car</t>
         </is>
       </c>
       <c r="D817" t="n">
@@ -35581,7 +35581,7 @@
       </c>
       <c r="C818" t="inlineStr">
         <is>
-          <t>'domestic appliance'</t>
+          <t>domestic appliance</t>
         </is>
       </c>
       <c r="D818" t="n">
@@ -35753,7 +35753,7 @@
       </c>
       <c r="C822" t="inlineStr">
         <is>
-          <t>'new car'</t>
+          <t>new car</t>
         </is>
       </c>
       <c r="D822" t="n">
@@ -35882,7 +35882,7 @@
       </c>
       <c r="C825" t="inlineStr">
         <is>
-          <t>'new car'</t>
+          <t>new car</t>
         </is>
       </c>
       <c r="D825" t="n">
@@ -35968,7 +35968,7 @@
       </c>
       <c r="C827" t="inlineStr">
         <is>
-          <t>'new car'</t>
+          <t>new car</t>
         </is>
       </c>
       <c r="D827" t="n">
@@ -36011,7 +36011,7 @@
       </c>
       <c r="C828" t="inlineStr">
         <is>
-          <t>'new car'</t>
+          <t>new car</t>
         </is>
       </c>
       <c r="D828" t="n">
@@ -36097,7 +36097,7 @@
       </c>
       <c r="C830" t="inlineStr">
         <is>
-          <t>'used car'</t>
+          <t>used car</t>
         </is>
       </c>
       <c r="D830" t="n">
@@ -36226,7 +36226,7 @@
       </c>
       <c r="C833" t="inlineStr">
         <is>
-          <t>'new car'</t>
+          <t>new car</t>
         </is>
       </c>
       <c r="D833" t="n">
@@ -36398,7 +36398,7 @@
       </c>
       <c r="C837" t="inlineStr">
         <is>
-          <t>'new car'</t>
+          <t>new car</t>
         </is>
       </c>
       <c r="D837" t="n">
@@ -36527,7 +36527,7 @@
       </c>
       <c r="C840" t="inlineStr">
         <is>
-          <t>'used car'</t>
+          <t>used car</t>
         </is>
       </c>
       <c r="D840" t="n">
@@ -36656,7 +36656,7 @@
       </c>
       <c r="C843" t="inlineStr">
         <is>
-          <t>'used car'</t>
+          <t>used car</t>
         </is>
       </c>
       <c r="D843" t="n">
@@ -36871,7 +36871,7 @@
       </c>
       <c r="C848" t="inlineStr">
         <is>
-          <t>'new car'</t>
+          <t>new car</t>
         </is>
       </c>
       <c r="D848" t="n">
@@ -36914,7 +36914,7 @@
       </c>
       <c r="C849" t="inlineStr">
         <is>
-          <t>'new car'</t>
+          <t>new car</t>
         </is>
       </c>
       <c r="D849" t="n">
@@ -37043,7 +37043,7 @@
       </c>
       <c r="C852" t="inlineStr">
         <is>
-          <t>'new car'</t>
+          <t>new car</t>
         </is>
       </c>
       <c r="D852" t="n">
@@ -37086,7 +37086,7 @@
       </c>
       <c r="C853" t="inlineStr">
         <is>
-          <t>'used car'</t>
+          <t>used car</t>
         </is>
       </c>
       <c r="D853" t="n">
@@ -37172,7 +37172,7 @@
       </c>
       <c r="C855" t="inlineStr">
         <is>
-          <t>'new car'</t>
+          <t>new car</t>
         </is>
       </c>
       <c r="D855" t="n">
@@ -37215,7 +37215,7 @@
       </c>
       <c r="C856" t="inlineStr">
         <is>
-          <t>'new car'</t>
+          <t>new car</t>
         </is>
       </c>
       <c r="D856" t="n">
@@ -37258,7 +37258,7 @@
       </c>
       <c r="C857" t="inlineStr">
         <is>
-          <t>'new car'</t>
+          <t>new car</t>
         </is>
       </c>
       <c r="D857" t="n">
@@ -37387,7 +37387,7 @@
       </c>
       <c r="C860" t="inlineStr">
         <is>
-          <t>'new car'</t>
+          <t>new car</t>
         </is>
       </c>
       <c r="D860" t="n">
@@ -37430,7 +37430,7 @@
       </c>
       <c r="C861" t="inlineStr">
         <is>
-          <t>'new car'</t>
+          <t>new car</t>
         </is>
       </c>
       <c r="D861" t="n">
@@ -37473,7 +37473,7 @@
       </c>
       <c r="C862" t="inlineStr">
         <is>
-          <t>'used car'</t>
+          <t>used car</t>
         </is>
       </c>
       <c r="D862" t="n">
@@ -37946,7 +37946,7 @@
       </c>
       <c r="C873" t="inlineStr">
         <is>
-          <t>'new car'</t>
+          <t>new car</t>
         </is>
       </c>
       <c r="D873" t="n">
@@ -38032,7 +38032,7 @@
       </c>
       <c r="C875" t="inlineStr">
         <is>
-          <t>'domestic appliance'</t>
+          <t>domestic appliance</t>
         </is>
       </c>
       <c r="D875" t="n">
@@ -38118,7 +38118,7 @@
       </c>
       <c r="C877" t="inlineStr">
         <is>
-          <t>'new car'</t>
+          <t>new car</t>
         </is>
       </c>
       <c r="D877" t="n">
@@ -38247,7 +38247,7 @@
       </c>
       <c r="C880" t="inlineStr">
         <is>
-          <t>'new car'</t>
+          <t>new car</t>
         </is>
       </c>
       <c r="D880" t="n">
@@ -38333,7 +38333,7 @@
       </c>
       <c r="C882" t="inlineStr">
         <is>
-          <t>'used car'</t>
+          <t>used car</t>
         </is>
       </c>
       <c r="D882" t="n">
@@ -38376,7 +38376,7 @@
       </c>
       <c r="C883" t="inlineStr">
         <is>
-          <t>'used car'</t>
+          <t>used car</t>
         </is>
       </c>
       <c r="D883" t="n">
@@ -38419,7 +38419,7 @@
       </c>
       <c r="C884" t="inlineStr">
         <is>
-          <t>'new car'</t>
+          <t>new car</t>
         </is>
       </c>
       <c r="D884" t="n">
@@ -38677,7 +38677,7 @@
       </c>
       <c r="C890" t="inlineStr">
         <is>
-          <t>'new car'</t>
+          <t>new car</t>
         </is>
       </c>
       <c r="D890" t="n">
@@ -38720,7 +38720,7 @@
       </c>
       <c r="C891" t="inlineStr">
         <is>
-          <t>'used car'</t>
+          <t>used car</t>
         </is>
       </c>
       <c r="D891" t="n">
@@ -38849,7 +38849,7 @@
       </c>
       <c r="C894" t="inlineStr">
         <is>
-          <t>'new car'</t>
+          <t>new car</t>
         </is>
       </c>
       <c r="D894" t="n">
@@ -38892,7 +38892,7 @@
       </c>
       <c r="C895" t="inlineStr">
         <is>
-          <t>'used car'</t>
+          <t>used car</t>
         </is>
       </c>
       <c r="D895" t="n">
@@ -38978,7 +38978,7 @@
       </c>
       <c r="C897" t="inlineStr">
         <is>
-          <t>'used car'</t>
+          <t>used car</t>
         </is>
       </c>
       <c r="D897" t="n">
@@ -39193,7 +39193,7 @@
       </c>
       <c r="C902" t="inlineStr">
         <is>
-          <t>'new car'</t>
+          <t>new car</t>
         </is>
       </c>
       <c r="D902" t="n">
@@ -39236,7 +39236,7 @@
       </c>
       <c r="C903" t="inlineStr">
         <is>
-          <t>'new car'</t>
+          <t>new car</t>
         </is>
       </c>
       <c r="D903" t="n">
@@ -39279,7 +39279,7 @@
       </c>
       <c r="C904" t="inlineStr">
         <is>
-          <t>'used car'</t>
+          <t>used car</t>
         </is>
       </c>
       <c r="D904" t="n">
@@ -39451,7 +39451,7 @@
       </c>
       <c r="C908" t="inlineStr">
         <is>
-          <t>'new car'</t>
+          <t>new car</t>
         </is>
       </c>
       <c r="D908" t="n">
@@ -39537,7 +39537,7 @@
       </c>
       <c r="C910" t="inlineStr">
         <is>
-          <t>'used car'</t>
+          <t>used car</t>
         </is>
       </c>
       <c r="D910" t="n">
@@ -39580,7 +39580,7 @@
       </c>
       <c r="C911" t="inlineStr">
         <is>
-          <t>'new car'</t>
+          <t>new car</t>
         </is>
       </c>
       <c r="D911" t="n">
@@ -39881,7 +39881,7 @@
       </c>
       <c r="C918" t="inlineStr">
         <is>
-          <t>'used car'</t>
+          <t>used car</t>
         </is>
       </c>
       <c r="D918" t="n">
@@ -39924,7 +39924,7 @@
       </c>
       <c r="C919" t="inlineStr">
         <is>
-          <t>'new car'</t>
+          <t>new car</t>
         </is>
       </c>
       <c r="D919" t="n">
@@ -40182,7 +40182,7 @@
       </c>
       <c r="C925" t="inlineStr">
         <is>
-          <t>'new car'</t>
+          <t>new car</t>
         </is>
       </c>
       <c r="D925" t="n">
@@ -40268,7 +40268,7 @@
       </c>
       <c r="C927" t="inlineStr">
         <is>
-          <t>'new car'</t>
+          <t>new car</t>
         </is>
       </c>
       <c r="D927" t="n">
@@ -40354,7 +40354,7 @@
       </c>
       <c r="C929" t="inlineStr">
         <is>
-          <t>'used car'</t>
+          <t>used car</t>
         </is>
       </c>
       <c r="D929" t="n">
@@ -40440,7 +40440,7 @@
       </c>
       <c r="C931" t="inlineStr">
         <is>
-          <t>'new car'</t>
+          <t>new car</t>
         </is>
       </c>
       <c r="D931" t="n">
@@ -40569,7 +40569,7 @@
       </c>
       <c r="C934" t="inlineStr">
         <is>
-          <t>'new car'</t>
+          <t>new car</t>
         </is>
       </c>
       <c r="D934" t="n">
@@ -40870,7 +40870,7 @@
       </c>
       <c r="C941" t="inlineStr">
         <is>
-          <t>'used car'</t>
+          <t>used car</t>
         </is>
       </c>
       <c r="D941" t="n">
@@ -40913,7 +40913,7 @@
       </c>
       <c r="C942" t="inlineStr">
         <is>
-          <t>'new car'</t>
+          <t>new car</t>
         </is>
       </c>
       <c r="D942" t="n">
@@ -40956,7 +40956,7 @@
       </c>
       <c r="C943" t="inlineStr">
         <is>
-          <t>'new car'</t>
+          <t>new car</t>
         </is>
       </c>
       <c r="D943" t="n">
@@ -41042,7 +41042,7 @@
       </c>
       <c r="C945" t="inlineStr">
         <is>
-          <t>'new car'</t>
+          <t>new car</t>
         </is>
       </c>
       <c r="D945" t="n">
@@ -41128,7 +41128,7 @@
       </c>
       <c r="C947" t="inlineStr">
         <is>
-          <t>'new car'</t>
+          <t>new car</t>
         </is>
       </c>
       <c r="D947" t="n">
@@ -41214,7 +41214,7 @@
       </c>
       <c r="C949" t="inlineStr">
         <is>
-          <t>'new car'</t>
+          <t>new car</t>
         </is>
       </c>
       <c r="D949" t="n">
@@ -41429,7 +41429,7 @@
       </c>
       <c r="C954" t="inlineStr">
         <is>
-          <t>'used car'</t>
+          <t>used car</t>
         </is>
       </c>
       <c r="D954" t="n">
@@ -41515,7 +41515,7 @@
       </c>
       <c r="C956" t="inlineStr">
         <is>
-          <t>'new car'</t>
+          <t>new car</t>
         </is>
       </c>
       <c r="D956" t="n">
@@ -41687,7 +41687,7 @@
       </c>
       <c r="C960" t="inlineStr">
         <is>
-          <t>'new car'</t>
+          <t>new car</t>
         </is>
       </c>
       <c r="D960" t="n">
@@ -41816,7 +41816,7 @@
       </c>
       <c r="C963" t="inlineStr">
         <is>
-          <t>'new car'</t>
+          <t>new car</t>
         </is>
       </c>
       <c r="D963" t="n">
@@ -41859,7 +41859,7 @@
       </c>
       <c r="C964" t="inlineStr">
         <is>
-          <t>'new car'</t>
+          <t>new car</t>
         </is>
       </c>
       <c r="D964" t="n">
@@ -42160,7 +42160,7 @@
       </c>
       <c r="C971" t="inlineStr">
         <is>
-          <t>'new car'</t>
+          <t>new car</t>
         </is>
       </c>
       <c r="D971" t="n">
@@ -42246,7 +42246,7 @@
       </c>
       <c r="C973" t="inlineStr">
         <is>
-          <t>'new car'</t>
+          <t>new car</t>
         </is>
       </c>
       <c r="D973" t="n">
@@ -42289,7 +42289,7 @@
       </c>
       <c r="C974" t="inlineStr">
         <is>
-          <t>'new car'</t>
+          <t>new car</t>
         </is>
       </c>
       <c r="D974" t="n">
@@ -42547,7 +42547,7 @@
       </c>
       <c r="C980" t="inlineStr">
         <is>
-          <t>'new car'</t>
+          <t>new car</t>
         </is>
       </c>
       <c r="D980" t="n">
@@ -42590,7 +42590,7 @@
       </c>
       <c r="C981" t="inlineStr">
         <is>
-          <t>'new car'</t>
+          <t>new car</t>
         </is>
       </c>
       <c r="D981" t="n">
@@ -42719,7 +42719,7 @@
       </c>
       <c r="C984" t="inlineStr">
         <is>
-          <t>'new car'</t>
+          <t>new car</t>
         </is>
       </c>
       <c r="D984" t="n">
@@ -42762,7 +42762,7 @@
       </c>
       <c r="C985" t="inlineStr">
         <is>
-          <t>'used car'</t>
+          <t>used car</t>
         </is>
       </c>
       <c r="D985" t="n">
@@ -42977,7 +42977,7 @@
       </c>
       <c r="C990" t="inlineStr">
         <is>
-          <t>'used car'</t>
+          <t>used car</t>
         </is>
       </c>
       <c r="D990" t="n">
@@ -43235,7 +43235,7 @@
       </c>
       <c r="C996" t="inlineStr">
         <is>
-          <t>'new car'</t>
+          <t>new car</t>
         </is>
       </c>
       <c r="D996" t="n">
@@ -43321,7 +43321,7 @@
       </c>
       <c r="C998" t="inlineStr">
         <is>
-          <t>'used car'</t>
+          <t>used car</t>
         </is>
       </c>
       <c r="D998" t="n">
@@ -43450,7 +43450,7 @@
       </c>
       <c r="C1001" t="inlineStr">
         <is>
-          <t>'used car'</t>
+          <t>used car</t>
         </is>
       </c>
       <c r="D1001" t="n">

</xml_diff>